<commit_message>
Cone enemy agents with detection not working properly
</commit_message>
<xml_diff>
--- a/resources/Levels/LevelEditor.xlsx
+++ b/resources/Levels/LevelEditor.xlsx
@@ -61,161 +61,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="97">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFAC2626"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFAC2626"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFAC2626"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFAC2626"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="37">
     <dxf>
       <fill>
         <patternFill>
@@ -471,273 +317,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFAC2626"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFAC2626"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFAC2626"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFAC2626"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFAC2626"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFAC2626"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFAC2626"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFAC2626"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1025,7 +605,7 @@
   <dimension ref="A1:BH34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="BJ17" sqref="BJ17"/>
+      <selection activeCell="BJ38" sqref="BJ38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.85546875" defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1674,7 +1254,7 @@
         <v>2</v>
       </c>
       <c r="AG4" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AH4" s="1">
         <v>2</v>
@@ -1856,7 +1436,7 @@
         <v>2</v>
       </c>
       <c r="AG5" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="AH5" s="1">
         <v>2</v>
@@ -2136,7 +1716,7 @@
         <v>2</v>
       </c>
       <c r="E7" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F7" s="1">
         <v>2</v>
@@ -2318,7 +1898,7 @@
         <v>2</v>
       </c>
       <c r="E8" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F8" s="1">
         <v>2</v>
@@ -2802,10 +2382,10 @@
         <v>2</v>
       </c>
       <c r="AS10" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="AT10" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AU10" s="1">
         <v>2</v>
@@ -7220,17 +6800,71 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="R28">
-    <cfRule type="cellIs" dxfId="21" priority="22" operator="between">
+    <cfRule type="cellIs" dxfId="36" priority="37" operator="between">
       <formula>1</formula>
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO25">
-    <cfRule type="cellIs" dxfId="20" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="36" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A27:BH34 A20:L26 N20:BH26 A6:BH19 A4:Q5 AC4:BH5 A1:BH3">
+  <conditionalFormatting sqref="A27:BH34 A20:L26 N20:BH26 A4:Q5 A1:BH3 AC4:AF4 AH4:BH4 AC5:BH5 A6:BH6 A7:D7 F7:BH7 A8:BH9 A11:BH19 AU10:BH10 A10:AS10">
+    <cfRule type="cellIs" dxfId="34" priority="31" operator="equal">
+      <formula>6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="32" operator="between">
+      <formula>3</formula>
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="33" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="31" priority="34" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="35" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M21:M26">
+    <cfRule type="cellIs" dxfId="29" priority="26" operator="equal">
+      <formula>6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="27" operator="between">
+      <formula>3</formula>
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="28" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="29" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="30" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M20">
+    <cfRule type="cellIs" dxfId="24" priority="21" operator="equal">
+      <formula>6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="22" operator="between">
+      <formula>3</formula>
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="23" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="24" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="25" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R4:AB5">
     <cfRule type="cellIs" dxfId="19" priority="16" operator="equal">
       <formula>6</formula>
     </cfRule>
@@ -7248,7 +6882,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M21:M26">
+  <conditionalFormatting sqref="AG4">
     <cfRule type="cellIs" dxfId="14" priority="11" operator="equal">
       <formula>6</formula>
     </cfRule>
@@ -7266,7 +6900,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M20">
+  <conditionalFormatting sqref="E7">
     <cfRule type="cellIs" dxfId="9" priority="6" operator="equal">
       <formula>6</formula>
     </cfRule>
@@ -7284,7 +6918,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R4:AB5">
+  <conditionalFormatting sqref="AT10">
     <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>6</formula>
     </cfRule>

</xml_diff>

<commit_message>
Win/Lose game and menus
</commit_message>
<xml_diff>
--- a/resources/Levels/LevelEditor.xlsx
+++ b/resources/Levels/LevelEditor.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pol_b\Documents\Enti\SourceTree\IA\PracticaFinal\resources\Levels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ENTI\5º Semestre\Tecnicas de inteligencia artificial para videojuegos\Demos\PracticaFinal_IA\resources\Levels\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -605,7 +605,7 @@
   <dimension ref="A1:BH34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Z16" sqref="Z16"/>
+      <selection activeCell="B4" sqref="A1:BH34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.85546875" defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -797,13 +797,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1">
         <v>3</v>
-      </c>
-      <c r="C2" s="1">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1">
-        <v>2</v>
       </c>
       <c r="E2" s="1">
         <v>3</v>
@@ -1161,7 +1161,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1">
         <v>2</v>

</xml_diff>